<commit_message>
chore: Remove unnecessary code and export app for Netlify Functions
</commit_message>
<xml_diff>
--- a/form-data.xlsx
+++ b/form-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -701,9 +701,32 @@
         <v>po</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Shikuku Emmanuel</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Nabwana</v>
+      </c>
+      <c r="C14" t="str">
+        <v>CALATECH</v>
+      </c>
+      <c r="D14" t="str">
+        <v>agile</v>
+      </c>
+      <c r="E14" t="str">
+        <v>0757003013</v>
+      </c>
+      <c r="F14" t="str">
+        <v>enshikuku@gmail.com</v>
+      </c>
+      <c r="G14" t="str">
+        <v>gfgfg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: Update registration page layout, style.css, and add export functionality
</commit_message>
<xml_diff>
--- a/form-data.xlsx
+++ b/form-data.xlsx
@@ -397,32 +397,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>first-name</v>
+        <v>First_Name</v>
       </c>
       <c r="B1" t="str">
-        <v>last-name</v>
+        <v>Last_Name</v>
       </c>
       <c r="C1" t="str">
-        <v>company</v>
+        <v>Company</v>
       </c>
       <c r="D1" t="str">
-        <v>industry</v>
+        <v>Industry</v>
       </c>
       <c r="E1" t="str">
-        <v>phone</v>
-      </c>
-      <c r="F1" t="str">
-        <v>email</v>
-      </c>
-      <c r="G1" t="str">
-        <v>department</v>
+        <v>Job_Title</v>
       </c>
     </row>
     <row r="2">
@@ -433,19 +427,13 @@
         <v>Nabwana</v>
       </c>
       <c r="C2" t="str">
-        <v>CALATECH</v>
+        <v>Agile</v>
       </c>
       <c r="D2" t="str">
-        <v>das</v>
+        <v>Marketing</v>
       </c>
       <c r="E2" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F2" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G2" t="str">
-        <v>das</v>
+        <v>Online Marketer</v>
       </c>
     </row>
     <row r="3">
@@ -456,19 +444,13 @@
         <v>Nabwana</v>
       </c>
       <c r="C3" t="str">
-        <v>CALATECH</v>
+        <v>Agile</v>
       </c>
       <c r="D3" t="str">
-        <v>das</v>
+        <v>HR</v>
       </c>
       <c r="E3" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F3" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G3" t="str">
-        <v>das</v>
+        <v>HR manager</v>
       </c>
     </row>
     <row r="4">
@@ -479,19 +461,13 @@
         <v>Nabwana</v>
       </c>
       <c r="C4" t="str">
-        <v>CALATECH</v>
+        <v>Agile</v>
       </c>
       <c r="D4" t="str">
-        <v>das</v>
+        <v>HR</v>
       </c>
       <c r="E4" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F4" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G4" t="str">
-        <v>das</v>
+        <v>HR manager</v>
       </c>
     </row>
     <row r="5">
@@ -502,19 +478,13 @@
         <v>Nabwana</v>
       </c>
       <c r="C5" t="str">
-        <v>CALATECH</v>
+        <v>Agile</v>
       </c>
       <c r="D5" t="str">
-        <v>das</v>
+        <v>HR</v>
       </c>
       <c r="E5" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F5" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G5" t="str">
-        <v>das</v>
+        <v>HR manager</v>
       </c>
     </row>
     <row r="6">
@@ -525,208 +495,18 @@
         <v>Nabwana</v>
       </c>
       <c r="C6" t="str">
-        <v>CALATECH</v>
+        <v>Agile</v>
       </c>
       <c r="D6" t="str">
-        <v>das</v>
+        <v>HR</v>
       </c>
       <c r="E6" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F6" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G6" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C7" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D7" t="str">
-        <v>das</v>
-      </c>
-      <c r="E7" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F7" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G7" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C8" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D8" t="str">
-        <v>das</v>
-      </c>
-      <c r="E8" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F8" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G8" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C9" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D9" t="str">
-        <v>das</v>
-      </c>
-      <c r="E9" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F9" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G9" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C10" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D10" t="str">
-        <v>das</v>
-      </c>
-      <c r="E10" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F10" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G10" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C11" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D11" t="str">
-        <v>das</v>
-      </c>
-      <c r="E11" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F11" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G11" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C12" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D12" t="str">
-        <v>das</v>
-      </c>
-      <c r="E12" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F12" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G12" t="str">
-        <v>das</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C13" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D13" t="str">
-        <v>agile</v>
-      </c>
-      <c r="E13" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F13" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G13" t="str">
-        <v>po</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Shikuku Emmanuel</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Nabwana</v>
-      </c>
-      <c r="C14" t="str">
-        <v>CALATECH</v>
-      </c>
-      <c r="D14" t="str">
-        <v>agile</v>
-      </c>
-      <c r="E14" t="str">
-        <v>0757003013</v>
-      </c>
-      <c r="F14" t="str">
-        <v>enshikuku@gmail.com</v>
-      </c>
-      <c r="G14" t="str">
-        <v>gfgfg</v>
+        <v>HR manager</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: Update style.css and app.js, and improve registration page layout
</commit_message>
<xml_diff>
--- a/form-data.xlsx
+++ b/form-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -521,9 +521,26 @@
         <v>HR manager</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Shikuku Emmanuel</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Nabwana</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Kenyan</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Marketing</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Marketing</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>